<commit_message>
Oppdatert budsjett og skulder ledd
</commit_message>
<xml_diff>
--- a/Budsjett.xlsx
+++ b/Budsjett.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dngmo\Documents\BachelorProsjekt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UIA\Bachelor\BachelorProsjekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0BB6CC7C-DB94-46FE-BC56-F9BD0F522EF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046B96FA-F636-46A1-A780-062F6FF8E32C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7ECF43A6-1848-4FDA-8461-36822067C1B7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7ECF43A6-1848-4FDA-8461-36822067C1B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>Part number</t>
   </si>
@@ -59,40 +59,82 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>SKU:FIT0185</t>
-  </si>
-  <si>
-    <t>1 krage, 2 skulder rot, 1 skulder lateral, 1 albue</t>
-  </si>
-  <si>
-    <t>sm_m08t60h10</t>
-  </si>
-  <si>
-    <t>sm_m08t80h10</t>
-  </si>
-  <si>
-    <t>sm_m08t15h06</t>
-  </si>
-  <si>
-    <t>PART LIST UP UNTILL ELBOW JOINT</t>
-  </si>
-  <si>
-    <t>1 skulder, 1 cut skulder lateral</t>
-  </si>
-  <si>
-    <t>1 krage, 1albue</t>
-  </si>
-  <si>
-    <t>Bearing</t>
-  </si>
-  <si>
-    <t>Gear</t>
-  </si>
-  <si>
-    <t>sm = self made</t>
-  </si>
-  <si>
-    <t>DDLF1910ZZRA5P24LY121</t>
+    <t>NFP-5840-31ZYS-D</t>
+  </si>
+  <si>
+    <t>NFP-GA32Y-31ZY-EN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Motor </t>
+  </si>
+  <si>
+    <t>NFP-GA20Y-180</t>
+  </si>
+  <si>
+    <t>Microdcmotor</t>
+  </si>
+  <si>
+    <t>Place</t>
+  </si>
+  <si>
+    <t>RS component</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>Selfmade</t>
+  </si>
+  <si>
+    <t>Pulley</t>
+  </si>
+  <si>
+    <t>Idler</t>
+  </si>
+  <si>
+    <t>Miniature ball bearing</t>
+  </si>
+  <si>
+    <t>Thrust bearing</t>
+  </si>
+  <si>
+    <t>Roller bearing</t>
+  </si>
+  <si>
+    <t>608-2RS</t>
+  </si>
+  <si>
+    <t>146-9289</t>
+  </si>
+  <si>
+    <t>Motor controller</t>
+  </si>
+  <si>
+    <t>Buck converter</t>
+  </si>
+  <si>
+    <t>Position sensor</t>
+  </si>
+  <si>
+    <t>I2C level converter</t>
+  </si>
+  <si>
+    <t>HTD Timing Belt</t>
+  </si>
+  <si>
+    <t>pulley_20_5m__09_8</t>
+  </si>
+  <si>
+    <t>pulley_40_5m__09_10</t>
+  </si>
+  <si>
+    <t>idler_09_6</t>
+  </si>
+  <si>
+    <t>Frakt</t>
+  </si>
+  <si>
+    <t>Biltema</t>
   </si>
 </sst>
 </file>
@@ -108,15 +150,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -124,29 +172,18 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -166,7 +203,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -454,7 +491,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -462,20 +499,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77625910-4474-448E-B890-7D3021245776}">
-  <dimension ref="A2:I15"/>
+  <dimension ref="A2:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="43" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -494,161 +535,295 @@
       <c r="G2" t="s">
         <v>6</v>
       </c>
-      <c r="I2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="1" t="s">
-        <v>7</v>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
       </c>
       <c r="D3">
-        <v>300</v>
+        <v>260</v>
       </c>
       <c r="E3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F3">
         <f>D3*E3</f>
-        <v>1500</v>
-      </c>
-      <c r="G3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
+        <v>520</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
       <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>195</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ref="F4:F5" si="0">D4*E4</f>
+        <v>390</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-      <c r="F4">
-        <f t="shared" ref="F4:F15" si="0">D4*E4</f>
-        <v>0</v>
-      </c>
-      <c r="G4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
       <c r="D5">
-        <v>0</v>
+        <v>115</v>
       </c>
       <c r="E5">
         <v>2</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>5</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
         <v>18</v>
       </c>
-      <c r="C7" t="s">
-        <v>15</v>
-      </c>
       <c r="D7">
-        <v>130</v>
+        <v>34</v>
       </c>
       <c r="E7">
         <v>10</v>
       </c>
       <c r="F7">
-        <f t="shared" si="0"/>
-        <v>1300</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <f>D7*E7</f>
+        <v>340</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="3">
+        <v>51100</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8">
+        <v>63</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
       <c r="F8">
-        <f t="shared" si="0"/>
+        <f>D8*E8</f>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9">
+        <v>42</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <f>D9*E9</f>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10">
+        <v>100</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <f>D10*E10</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18">
+        <v>146</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18">
+        <f>D18*E18</f>
+        <v>292</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+      <c r="C19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19">
+        <v>166</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <f>D19*E19</f>
+        <v>166</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+      <c r="C20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20">
+        <v>122</v>
+      </c>
+      <c r="E20">
+        <v>5</v>
+      </c>
+      <c r="F20">
+        <f>D20*E20</f>
+        <v>610</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="C21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21">
+        <v>111</v>
+      </c>
+      <c r="E21">
+        <v>2</v>
+      </c>
+      <c r="F21">
+        <f>D21*E21</f>
+        <v>222</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F22">
+        <v>200</v>
+      </c>
+      <c r="G22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F9">
-        <f t="shared" si="0"/>
+      <c r="E24">
+        <v>2</v>
+      </c>
+      <c r="F24">
+        <f>D24*E24</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F10">
-        <f t="shared" si="0"/>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="1"/>
+      <c r="B25" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F11">
-        <f t="shared" si="0"/>
+      <c r="E25">
+        <v>2</v>
+      </c>
+      <c r="F25">
+        <f>D25*E25</f>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F12">
-        <f t="shared" si="0"/>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="1"/>
+      <c r="B26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F13">
-        <f t="shared" si="0"/>
+      <c r="E26">
+        <v>2</v>
+      </c>
+      <c r="F26">
+        <f t="shared" ref="F25:F26" si="1">D26*E26</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F15">
-        <f t="shared" si="0"/>
-        <v>0</v>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F29">
+        <f>SUM(F3:F21)</f>
+        <v>3180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Testplate til wormgear motor
</commit_message>
<xml_diff>
--- a/Budsjett.xlsx
+++ b/Budsjett.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UIA\Bachelor\BachelorProsjekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046B96FA-F636-46A1-A780-062F6FF8E32C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E65E91-31CA-46A2-9227-9E7E3BDB8B75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7ECF43A6-1848-4FDA-8461-36822067C1B7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>Part number</t>
   </si>
@@ -129,9 +129,6 @@
   </si>
   <si>
     <t>idler_09_6</t>
-  </si>
-  <si>
-    <t>Frakt</t>
   </si>
   <si>
     <t>Biltema</t>
@@ -179,7 +176,7 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -499,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77625910-4474-448E-B890-7D3021245776}">
-  <dimension ref="A2:G29"/>
+  <dimension ref="A2:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -595,219 +592,191 @@
         <v>230</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F6">
+        <f>SUM(F3:F5)</f>
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B9" t="s">
         <v>21</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C9" t="s">
         <v>18</v>
       </c>
-      <c r="D7">
+      <c r="D9">
         <v>34</v>
       </c>
-      <c r="E7">
+      <c r="E9">
         <v>10</v>
-      </c>
-      <c r="F7">
-        <f>D7*E7</f>
-        <v>340</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
-      <c r="B8" s="3">
-        <v>51100</v>
-      </c>
-      <c r="C8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8">
-        <v>63</v>
-      </c>
-      <c r="E8">
-        <v>2</v>
-      </c>
-      <c r="F8">
-        <f>D8*E8</f>
-        <v>126</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
-      <c r="B9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9">
-        <v>42</v>
-      </c>
-      <c r="E9">
-        <v>2</v>
       </c>
       <c r="F9">
         <f>D9*E9</f>
-        <v>84</v>
+        <v>340</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
+      <c r="B10" s="3">
+        <v>51100</v>
+      </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D10">
-        <v>100</v>
+        <v>63</v>
       </c>
       <c r="E10">
         <v>2</v>
       </c>
       <c r="F10">
         <f>D10*E10</f>
-        <v>200</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11">
+        <v>42</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <f>D11*E11</f>
+        <v>84</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12">
+        <v>100</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12">
+        <f>D12*E12</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+      <c r="F13">
+        <f>SUM(F9:F12)</f>
+        <v>750</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
+      <c r="A14" s="1"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
+      <c r="A16" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="1"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C20" t="s">
         <v>23</v>
       </c>
-      <c r="D18">
+      <c r="D20">
         <v>146</v>
       </c>
-      <c r="E18">
-        <v>2</v>
-      </c>
-      <c r="F18">
-        <f>D18*E18</f>
-        <v>292</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
-      <c r="C19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19">
-        <v>166</v>
-      </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-      <c r="F19">
-        <f>D19*E19</f>
-        <v>166</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
-      <c r="C20" t="s">
-        <v>25</v>
-      </c>
-      <c r="D20">
-        <v>122</v>
-      </c>
       <c r="E20">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F20">
         <f>D20*E20</f>
-        <v>610</v>
+        <v>292</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="C21" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D21">
-        <v>111</v>
+        <v>166</v>
       </c>
       <c r="E21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F21">
         <f>D21*E21</f>
+        <v>166</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+      <c r="C22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22">
+        <v>122</v>
+      </c>
+      <c r="E22">
+        <v>5</v>
+      </c>
+      <c r="F22">
+        <f>D22*E22</f>
+        <v>610</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+      <c r="C23" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23">
+        <v>111</v>
+      </c>
+      <c r="E23">
+        <v>2</v>
+      </c>
+      <c r="F23">
+        <f>D23*E23</f>
         <v>222</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="F22">
-        <v>200</v>
-      </c>
-      <c r="G22" t="s">
-        <v>31</v>
-      </c>
-    </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
+      <c r="F24">
+        <v>1830</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B26" t="s">
         <v>29</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C26" t="s">
         <v>16</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <v>2</v>
-      </c>
-      <c r="F24">
-        <f>D24*E24</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="1"/>
-      <c r="B25" t="s">
-        <v>28</v>
-      </c>
-      <c r="C25" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25">
-        <v>2</v>
-      </c>
-      <c r="F25">
-        <f>D25*E25</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="1"/>
-      <c r="B26" t="s">
-        <v>30</v>
-      </c>
-      <c r="C26" t="s">
-        <v>17</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -816,14 +785,52 @@
         <v>2</v>
       </c>
       <c r="F26">
-        <f t="shared" ref="F25:F26" si="1">D26*E26</f>
+        <f>D26*E26</f>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="F29">
-        <f>SUM(F3:F21)</f>
-        <v>3180</v>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="1"/>
+      <c r="B27" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
+      <c r="F27">
+        <f>D27*E27</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="1"/>
+      <c r="B28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+      <c r="F28">
+        <f t="shared" ref="F28" si="1">D28*E28</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F31">
+        <f>F6+F13+F24</f>
+        <v>3720</v>
       </c>
     </row>
   </sheetData>

</xml_diff>